<commit_message>
avg height math function found
</commit_message>
<xml_diff>
--- a/abr-library/documentation/ALTEZZA ALBERO MEDIO.xlsx
+++ b/abr-library/documentation/ALTEZZA ALBERO MEDIO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NN</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>#CAMPIONE</t>
+  </si>
+  <si>
+    <t>h=OGRANDE(log)</t>
   </si>
 </sst>
 </file>
@@ -200,10 +203,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$A$2:$A$17</c:f>
+              <c:f>Foglio1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -211,103 +214,115 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1024</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2000</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42300</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65536</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>130000</c:v>
+                  <c:v>3876</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>131072</c:v>
+                  <c:v>19380</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>480456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$B$2:$B$17</c:f>
+              <c:f>Foglio1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.048</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3.34</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
-                  <c:v>5.04</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.024</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.32</c:v>
+                  <c:v>4.96</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.627000000000001</c:v>
+                  <c:v>6.5519999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.215999999999999</c:v>
+                  <c:v>6.6379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.725000000000001</c:v>
+                  <c:v>7.61</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.417000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22.175999999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23.838000000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>36.253</c:v>
+                  <c:v>8.0739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>8.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>8.0779999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
+                  <c:v>8.0299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39.225000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="#,##0">
-                  <c:v>42.555</c:v>
+                  <c:v>8.0730000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43.283000000000001</c:v>
+                  <c:v>8.07</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -391,10 +406,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$A$2:$A$17</c:f>
+              <c:f>Foglio1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -402,56 +417,62 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1024</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2000</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42300</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65536</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>130000</c:v>
+                  <c:v>3876</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>131072</c:v>
+                  <c:v>19380</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>480456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$C$2:$C$17</c:f>
+              <c:f>Foglio1!$C$2:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -459,46 +480,52 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.67</c:v>
+                  <c:v>0.64089648984620129</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.68</c:v>
+                  <c:v>0.456148727930068</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.756</c:v>
+                  <c:v>0.42379109089234779</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8640000000000001</c:v>
+                  <c:v>0.3421645001460597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9378333333333335</c:v>
+                  <c:v>0.27212042382440887</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0308571428571427</c:v>
+                  <c:v>0.27045239081923805</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0906250000000002</c:v>
+                  <c:v>0.21635516934803012</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1574444444444447</c:v>
+                  <c:v>0.16751555997301154</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2176</c:v>
+                  <c:v>0.15205322945581642</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1738527205338487</c:v>
+                  <c:v>0.12805242741183534</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3589359117989877</c:v>
+                  <c:v>0.10021778579334788</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4515625000000001</c:v>
+                  <c:v>8.7633207989039522E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.504981104200565</c:v>
+                  <c:v>5.6729727674998183E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5460588235294117</c:v>
+                  <c:v>3.9784548837988307E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9401525923645588E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2682002715542847E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,16 +1280,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>176212</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>481012</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1547,15 +1574,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,21 +1596,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="L2">
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1591,177 +1621,292 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C2:C17" si="0">B3/LOG(A3,2)</f>
+        <f>B3/POWER(LOG(A3,2),2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>B3/LOG(A3,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1.61</v>
+      </c>
+      <c r="C4">
+        <f>B4/POWER(LOG(A4,2),2)</f>
+        <v>0.64089648984620129</v>
+      </c>
+      <c r="D4">
+        <f>B4/LOG(A4,2)</f>
+        <v>1.0157969032500465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3.048</v>
+      </c>
+      <c r="C5">
+        <f>B5/POWER(LOG(A5,2),2)</f>
+        <v>0.456148727930068</v>
+      </c>
+      <c r="D5">
+        <f>B5/LOG(A5,2)</f>
+        <v>1.1791273564508828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>3.34</v>
+      </c>
+      <c r="C6">
+        <f>B6/POWER(LOG(A6,2),2)</f>
+        <v>0.42379109089234779</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D20" si="0">B6/LOG(A6,2)</f>
+        <v>1.189732004940794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>4.96</v>
+      </c>
+      <c r="C7">
+        <f>B7/POWER(LOG(A7,2),2)</f>
+        <v>0.3421645001460597</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.30274169378448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>6.5519999999999996</v>
+      </c>
+      <c r="C8">
+        <f>B8/POWER(LOG(A8,2),2)</f>
+        <v>0.27212042382440887</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.3352651485369964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>6.6379999999999999</v>
+      </c>
+      <c r="C9">
+        <f>B9/POWER(LOG(A9,2),2)</f>
+        <v>0.27045239081923805</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.3398742367319787</v>
+      </c>
+      <c r="O9" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>3.34</v>
-      </c>
-      <c r="C4">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>7.61</v>
+      </c>
+      <c r="C10">
+        <f>B10/POWER(LOG(A10,2),2)</f>
+        <v>0.21635516934803012</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5.04</v>
-      </c>
-      <c r="C5">
+        <v>1.2831456810271034</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>123</v>
+      </c>
+      <c r="B11">
+        <v>8.0739999999999998</v>
+      </c>
+      <c r="C11">
+        <f>B11/POWER(LOG(A11,2),2)</f>
+        <v>0.16751555997301154</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>7.024</v>
-      </c>
-      <c r="C6">
+        <v>1.1629792049826579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>155</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="C12">
+        <f>B12/POWER(LOG(A12,2),2)</f>
+        <v>0.15205322945581642</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.756</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>9.32</v>
-      </c>
-      <c r="C7">
+        <v>1.1063582137442296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>246</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+      <c r="C13">
+        <f>B13/POWER(LOG(A13,2),2)</f>
+        <v>0.12805242741183534</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.8640000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>64</v>
-      </c>
-      <c r="B8">
-        <v>11.627000000000001</v>
-      </c>
-      <c r="C8">
+        <v>1.0170582621624022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>495</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="C14">
+        <f>B14/POWER(LOG(A14,2),2)</f>
+        <v>0.10021778579334788</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>1.9378333333333335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>128</v>
-      </c>
-      <c r="B9">
-        <v>14.215999999999999</v>
-      </c>
-      <c r="C9">
+        <v>0.89707793413982895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>775</v>
+      </c>
+      <c r="B15">
+        <v>8.0730000000000004</v>
+      </c>
+      <c r="C15">
+        <f>B15/POWER(LOG(A15,2),2)</f>
+        <v>8.7633207989039522E-2</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
-        <v>2.0308571428571427</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>256</v>
-      </c>
-      <c r="B10">
-        <v>16.725000000000001</v>
-      </c>
-      <c r="C10">
+        <v>0.84110813103638238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3876</v>
+      </c>
+      <c r="B16">
+        <v>8.0609999999999999</v>
+      </c>
+      <c r="C16">
+        <f>B16/POWER(LOG(A16,2),2)</f>
+        <v>5.6729727674998183E-2</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
-        <v>2.0906250000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>512</v>
-      </c>
-      <c r="B11">
-        <v>19.417000000000002</v>
-      </c>
-      <c r="C11">
+        <v>0.67623837127758457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>19380</v>
+      </c>
+      <c r="B17">
+        <v>8.07</v>
+      </c>
+      <c r="C17">
+        <f>B17/POWER(LOG(A17,2),2)</f>
+        <v>3.9784548837988307E-2</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>2.1574444444444447</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1024</v>
-      </c>
-      <c r="B12">
-        <v>22.175999999999998</v>
-      </c>
-      <c r="C12">
+        <v>0.56662272203165809</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>96901</v>
+      </c>
+      <c r="B18">
+        <v>8.0670000000000002</v>
+      </c>
+      <c r="C18">
+        <f>B18/POWER(LOG(A18,2),2)</f>
+        <v>2.9401525923645588E-2</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
-        <v>2.2176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2000</v>
-      </c>
-      <c r="B13">
-        <v>23.838000000000001</v>
-      </c>
-      <c r="C13">
+        <v>0.48701345938900803</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>480456</v>
+      </c>
+      <c r="B19">
+        <v>8.08</v>
+      </c>
+      <c r="C19">
+        <f>B19/POWER(LOG(A19,2),2)</f>
+        <v>2.2682002715542847E-2</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
-        <v>2.1738527205338487</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>42300</v>
-      </c>
-      <c r="B14">
-        <v>36.253</v>
-      </c>
-      <c r="C14">
+        <v>0.42810113517904408</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>A18*10</f>
+        <v>969010</v>
+      </c>
+      <c r="B20">
+        <v>8.0679999999999996</v>
+      </c>
+      <c r="C20">
+        <f>B20/POWER(LOG(A20,2),2)</f>
+        <v>2.040160707664759E-2</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="0"/>
-        <v>2.3589359117989877</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>65536</v>
-      </c>
-      <c r="B15">
-        <v>39.225000000000001</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>2.4515625000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>130000</v>
-      </c>
-      <c r="B16" s="1">
-        <v>42.555</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>2.504981104200565</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>131072</v>
-      </c>
-      <c r="B17">
-        <v>43.283000000000001</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>2.5460588235294117</v>
-      </c>
+        <v>0.40570945995181423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:C17">

</xml_diff>